<commit_message>
fixed bugs of gru
</commit_message>
<xml_diff>
--- a/src/test/gru_example.xlsx
+++ b/src/test/gru_example.xlsx
@@ -655,7 +655,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1002,12 +1002,12 @@
         <v>1.2048242148098252</v>
       </c>
       <c r="P19" s="1">
-        <f>$J$4*G8+$K$4*G9+$L$4*G10+$M$4*G11+M19*($A$27*P8+$B$27*P9)+G14</f>
-        <v>1.2467771737822866</v>
+        <f>$J$4*G8+$K$4*G9+$L$4*G10+$M$4*G11+M23*($A$27*P8+$B$27*P9)+G14</f>
+        <v>1.1575880379320349</v>
       </c>
       <c r="Q19" s="1">
-        <f>$J$4*H8+$K$4*H9+$L$4*H10+$M$4*H11+N19*($A$27*Q8+$B$27*Q9)+H14</f>
-        <v>1.2467771737822866</v>
+        <f>$J$4*H8+$K$4*H9+$L$4*H10+$M$4*H11+N23*($A$27*Q8+$B$27*Q9)+H14</f>
+        <v>1.1575880379320349</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1052,12 +1052,12 @@
         <v>1.2048242148098252</v>
       </c>
       <c r="P20" s="1">
-        <f>$J$5*G8+$K$5*G9+$L$5*G10+$M$5*G11+M20*($A$28*P8+$B$28*P9)+G15</f>
-        <v>1.2467771737822866</v>
+        <f>$J$5*G8+$K$5*G9+$L$5*G10+$M$5*G11+M24*($A$28*P8+$B$28*P9)+G15</f>
+        <v>1.1575880379320349</v>
       </c>
       <c r="Q20" s="1">
-        <f>$J$5*H8+$K$5*H9+$L$5*H10+$M$5*H11+N20*($A$28*Q8+$B$28*Q9)+H15</f>
-        <v>1.2467771737822866</v>
+        <f>$J$5*H8+$K$5*H9+$L$5*H10+$M$5*H11+N24*($A$28*Q8+$B$28*Q9)+H15</f>
+        <v>1.1575880379320349</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1108,11 +1108,11 @@
       </c>
       <c r="P23" s="1">
         <f>(EXP(P19)-EXP(-P19))/(EXP(P19)+EXP(-P19))</f>
-        <v>0.8473774372713837</v>
+        <v>0.82025228036838227</v>
       </c>
       <c r="Q23" s="1">
         <f>(EXP(Q19)-EXP(-Q19))/(EXP(Q19)+EXP(-Q19))</f>
-        <v>0.8473774372713837</v>
+        <v>0.82025228036838227</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1158,11 +1158,11 @@
       </c>
       <c r="P24" s="1">
         <f>(EXP(P20)-EXP(-P20))/(EXP(P20)+EXP(-P20))</f>
-        <v>0.8473774372713837</v>
+        <v>0.82025228036838227</v>
       </c>
       <c r="Q24" s="1">
         <f>(EXP(Q20)-EXP(-Q20))/(EXP(Q20)+EXP(-Q20))</f>
-        <v>0.8473774372713837</v>
+        <v>0.82025228036838227</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1190,11 +1190,11 @@
       </c>
       <c r="J27" s="1">
         <f>(1-J23)*P23+J23*A27</f>
-        <v>0.35300863576693281</v>
+        <v>0.34675308287491935</v>
       </c>
       <c r="K27" s="1">
         <f>(1-K23)*Q23+K23*B27</f>
-        <v>0.35300863576693281</v>
+        <v>0.34675308287491935</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1208,11 +1208,11 @@
       </c>
       <c r="J28" s="1">
         <f>(1-J24)*P24+J24*A28</f>
-        <v>0.35300863576693281</v>
+        <v>0.34675308287491935</v>
       </c>
       <c r="K28" s="1">
         <f>(1-K24)*Q24+K24*B28</f>
-        <v>0.35300863576693281</v>
+        <v>0.34675308287491935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>